<commit_message>
Added comments and collections
</commit_message>
<xml_diff>
--- a/Laudobele Telma Testesanas Dokumentacija.xlsx
+++ b/Laudobele Telma Testesanas Dokumentacija.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telmy\OneDrive\school\final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F4E348-BD32-4421-9D68-0604B708297E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B748E6DB-0398-454A-BE8F-8DA34E74FCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
-    <workbookView minimized="1" xWindow="15750" yWindow="345" windowWidth="14430" windowHeight="15600" xr2:uid="{208A1C89-2B51-4F5D-9342-8A0EBFA0572C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="15600" activeTab="3" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="181">
   <si>
     <t>Sothoth Press</t>
   </si>
@@ -348,13 +347,7 @@
     <t>TP.BB.SES.03.</t>
   </si>
   <si>
-    <t>TP.S.I.</t>
-  </si>
-  <si>
     <t>Visu stāstu saņemšana no datubāzes</t>
-  </si>
-  <si>
-    <t>Atvērta tīmekļvietne</t>
   </si>
   <si>
     <t>Telma Ļaudobele</t>
@@ -464,9 +457,6 @@
     <t>TP.BB.SES.04.</t>
   </si>
   <si>
-    <t>Reģistrēšanās tīmekļvietnē ar pareiziem datiem</t>
-  </si>
-  <si>
     <t>Lietotājs tiek ielogots (izveidota sesijas sīkdatne) un aizsūtīts uz sākumlapu</t>
   </si>
   <si>
@@ -516,6 +506,84 @@
   </si>
   <si>
     <t>TZ.14.</t>
+  </si>
+  <si>
+    <t>Ielogošanās tīmekļvietnē ar nepareiziem datiem</t>
+  </si>
+  <si>
+    <t>PR.SES.04.</t>
+  </si>
+  <si>
+    <t>PR.SES.05.</t>
+  </si>
+  <si>
+    <t>Reģistrēšanās tīmekļvietnē ar nesakrītošām parolēm</t>
+  </si>
+  <si>
+    <t>Reģistrēšanās tīmekļvietnē neievadot datus</t>
+  </si>
+  <si>
+    <t>PR.SES.06.</t>
+  </si>
+  <si>
+    <t>Reģistrēšanās tīmekļvietnē ievadot nepieņemamus datus</t>
+  </si>
+  <si>
+    <t>Reģistrēšanās tīmekļvietnē ar pieņemamiem datiem</t>
+  </si>
+  <si>
+    <t>PR.SES.07.</t>
+  </si>
+  <si>
+    <t>TP.BB.SES.08.</t>
+  </si>
+  <si>
+    <t>2023.05.25</t>
+  </si>
+  <si>
+    <t>TZ.15.</t>
+  </si>
+  <si>
+    <t>TP.WB.S.I.01.</t>
+  </si>
+  <si>
+    <t>TP.WB.S.I.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.I.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.R.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.DZE.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.PUB.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.PAS.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.IER.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.IES.01.</t>
+  </si>
+  <si>
+    <t>When editing story publicize value is opposite</t>
+  </si>
+  <si>
+    <t>Remove "anonymous" option in documentation</t>
+  </si>
+  <si>
+    <t>CREATE A PUBLIC VIEW PROFILE PAGE</t>
+  </si>
+  <si>
+    <t>CREATE ADMIN PANEL</t>
+  </si>
+  <si>
+    <t>COLLECTION IN POST</t>
   </si>
 </sst>
 </file>
@@ -713,26 +781,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -748,6 +801,21 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1071,9 +1139,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1083,34 +1148,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="18"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1129,25 +1194,25 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1316,13 +1381,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3B1B55-F27C-465D-A977-BEEFFB3E0A70}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
-    </sheetView>
-    <sheetView zoomScaleNormal="100" workbookViewId="1">
-      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1354,10 +1416,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1371,7 +1433,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1379,7 +1441,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1387,104 +1449,114 @@
         <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="9"/>
+      <c r="A9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="9"/>
+      <c r="A18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="9"/>
+      <c r="A20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B22" s="9"/>
     </row>
@@ -1495,12 +1567,34 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B24" s="9"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="9"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1512,65 +1606,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{375F4E7E-8B48-4B59-97CF-C569B418CF30}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A5" sqref="A5:A7"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="36" style="14" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="47.140625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" style="14" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="24.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="36" style="11" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="47.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1583,10 +1674,10 @@
         <v>83</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>85</v>
@@ -1599,32 +1690,32 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1632,104 +1723,113 @@
       <c r="A6" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>36</v>
+        <v>123</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>36</v>
+        <v>123</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
-        <v>140</v>
+      <c r="D8" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="14" t="s">
-        <v>41</v>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
+      <c r="H9" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
+      <c r="H10" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B11" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
+      <c r="H11" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -1748,7 +1848,10 @@
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="8"/>
@@ -1756,52 +1859,25 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="14" t="s">
-        <v>43</v>
+      <c r="H14" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="8"/>
@@ -1809,13 +1885,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="8"/>
@@ -1823,13 +1901,15 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="8"/>
@@ -1837,13 +1917,15 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="8"/>
@@ -1851,13 +1933,15 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C22" s="8"/>
@@ -1865,13 +1949,15 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="8"/>
@@ -1879,13 +1965,15 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="8"/>
@@ -1893,19 +1981,19 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
@@ -1918,14 +2006,14 @@
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -1978,16 +2066,16 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
@@ -1997,19 +2085,19 @@
         <v>81</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="G34" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>18</v>
@@ -2026,14 +2114,14 @@
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
@@ -2046,38 +2134,46 @@
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
+      <c r="H39" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
+      <c r="A40" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -2086,24 +2182,23 @@
       <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
+      <c r="A42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
@@ -2116,14 +2211,14 @@
       <c r="H44" s="8"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
@@ -2154,6 +2249,36 @@
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2166,363 +2291,402 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5820504F-3397-4556-A5B2-F90EB4E6B868}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="15" style="18" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="18" customWidth="1"/>
-    <col min="5" max="6" width="25.140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="39.140625" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="15.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15" style="13" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="13" customWidth="1"/>
+    <col min="5" max="6" width="25.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="39.140625" style="13" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="8"/>
-      <c r="F4" s="19"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="21" t="s">
+      <c r="E6" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>132</v>
+      <c r="E7" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>129</v>
+      <c r="E9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="B15" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="B16" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="13" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C25" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C27" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C29" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="13" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fixes before preliminary showing
</commit_message>
<xml_diff>
--- a/Laudobele Telma Testesanas Dokumentacija.xlsx
+++ b/Laudobele Telma Testesanas Dokumentacija.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telmy\OneDrive\school\final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B748E6DB-0398-454A-BE8F-8DA34E74FCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA74A411-D219-4904-BF68-DC1FBB55BC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14430" windowHeight="15600" activeTab="3" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="183">
   <si>
     <t>Sothoth Press</t>
   </si>
@@ -584,6 +584,12 @@
   </si>
   <si>
     <t>COLLECTION IN POST</t>
+  </si>
+  <si>
+    <t>Reģistrēšanās tīmekļvietnē ievadot ar datubāzes vērtības sakrītošu ierakstu</t>
+  </si>
+  <si>
+    <t>Administratora panelis</t>
   </si>
 </sst>
 </file>
@@ -1381,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3B1B55-F27C-465D-A977-BEEFFB3E0A70}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1598,6 +1604,12 @@
         <v>71</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1608,8 +1620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{375F4E7E-8B48-4B59-97CF-C569B418CF30}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1831,13 +1843,23 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
+      <c r="H12" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
@@ -1848,9 +1870,6 @@
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>164</v>
-      </c>
       <c r="B14" s="11" t="s">
         <v>44</v>
       </c>
@@ -1859,9 +1878,6 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="1" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
@@ -2293,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5820504F-3397-4556-A5B2-F90EB4E6B868}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,9 +2635,7 @@
       <c r="E17" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>105</v>
-      </c>
+      <c r="F17" s="14"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2637,9 +2651,7 @@
       <c r="E18" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>105</v>
-      </c>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>

</xml_diff>

<commit_message>
Trying to make online hosting function again
</commit_message>
<xml_diff>
--- a/Laudobele Telma Testesanas Dokumentacija.xlsx
+++ b/Laudobele Telma Testesanas Dokumentacija.xlsx
@@ -8,10 +8,11 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telmy\OneDrive\school\final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0E005D-5B48-45EC-A265-1B9D741F280E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA4DCB4-B42D-4FB4-8474-6568DF986072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{56FCC86A-F332-49E3-B109-B86D43588ADF}"/>
+    <workbookView xWindow="-45" yWindow="0" windowWidth="16815" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
+    <workbookView xWindow="20955" yWindow="0" windowWidth="7800" windowHeight="15600" activeTab="1" xr2:uid="{56FCC86A-F332-49E3-B109-B86D43588ADF}"/>
+    <workbookView xWindow="16770" yWindow="60" windowWidth="4530" windowHeight="15480" firstSheet="2" activeTab="2" xr2:uid="{BCE1B89D-1D04-49A8-9071-0D8B36985319}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="364">
   <si>
     <t>Sothoth Press</t>
   </si>
@@ -587,9 +588,6 @@
     <t>TP.BB.S.DZE.02.</t>
   </si>
   <si>
-    <t>Stāsta rediģēšana izmainot aprakstu un sastāvu</t>
-  </si>
-  <si>
     <t>Stāsta dzēšanas atcelšana</t>
   </si>
   <si>
@@ -620,12 +618,6 @@
     <t>Lietotāja izveidoto stāstu uzrādīšana lietotājam</t>
   </si>
   <si>
-    <t>Ar lietotāju saistītie stāstu uzrādīšana administratoram</t>
-  </si>
-  <si>
-    <t>Ar lietotāju saistītie stāstu uzrādīšana lietotājam</t>
-  </si>
-  <si>
     <t>TP.BB.S.I.02.</t>
   </si>
   <si>
@@ -762,6 +754,387 @@
   </si>
   <si>
     <t>PR.KOL.08.</t>
+  </si>
+  <si>
+    <t>PR.A.01.</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Administrators</t>
+  </si>
+  <si>
+    <t>Administratora sadaļas ielāde</t>
+  </si>
+  <si>
+    <t>PR.A.02.</t>
+  </si>
+  <si>
+    <t>Administratora lomas apstiprināšana</t>
+  </si>
+  <si>
+    <t>PR.A.03.</t>
+  </si>
+  <si>
+    <t>Statistikas saņemšana no datubāzes</t>
+  </si>
+  <si>
+    <t>PR.A.04.</t>
+  </si>
+  <si>
+    <t>Lietotāja konta izdzēšana</t>
+  </si>
+  <si>
+    <t>PR.A.05.</t>
+  </si>
+  <si>
+    <t>Lietotāja konta lomas paaugstināšana uz administratoru</t>
+  </si>
+  <si>
+    <t>TP.BB.SES.09.</t>
+  </si>
+  <si>
+    <t>Ar lietotāju saistīto stāstu uzrādīšana lietotājam</t>
+  </si>
+  <si>
+    <t>Ar lietotāju saistīto stāstu uzrādīšana administratoram</t>
+  </si>
+  <si>
+    <t>Jauna stāsta izveide neievadot datus</t>
+  </si>
+  <si>
+    <t>PR.P.05.</t>
+  </si>
+  <si>
+    <t>PR.P.06.</t>
+  </si>
+  <si>
+    <t>Konta dzēšanas atcelšana</t>
+  </si>
+  <si>
+    <t>PR.S.09.</t>
+  </si>
+  <si>
+    <t>Konta dzēšana</t>
+  </si>
+  <si>
+    <t>TP.BB.P.I.01.</t>
+  </si>
+  <si>
+    <t>Publiskā profila lapas ielāde</t>
+  </si>
+  <si>
+    <t>TP.BB.P.I.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.P.I.03.</t>
+  </si>
+  <si>
+    <t>TP.BB.P.I.04.</t>
+  </si>
+  <si>
+    <t>TP.BB.P.R.01.</t>
+  </si>
+  <si>
+    <t>Publiskā profila datu rediģēšana</t>
+  </si>
+  <si>
+    <t>TP.BB.P.R.02.</t>
+  </si>
+  <si>
+    <t>Stāsta izdzēšana no profila skata</t>
+  </si>
+  <si>
+    <t>Jaunuma izdzēšana no profila skata</t>
+  </si>
+  <si>
+    <t>Komentāra izdzēšana no profila skata</t>
+  </si>
+  <si>
+    <t>TP.BB.P.R.03.</t>
+  </si>
+  <si>
+    <t>TP.BB.P.R.04.</t>
+  </si>
+  <si>
+    <t>TP.BB.P.DZE.01.</t>
+  </si>
+  <si>
+    <t>Datu rediģēšana no profila skata</t>
+  </si>
+  <si>
+    <t>PR.P.07.</t>
+  </si>
+  <si>
+    <t>TP.BB.P.DZE.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.J.I.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.J.I.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.J.IER.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.J.IES.01.</t>
+  </si>
+  <si>
+    <t>Jauna jaunuma ierakstīšana</t>
+  </si>
+  <si>
+    <t>Jauna jaunuma iesūtīšana datubāzē</t>
+  </si>
+  <si>
+    <t>TP.BB.J.DZE.01.</t>
+  </si>
+  <si>
+    <t>Jaunuma dzēšana</t>
+  </si>
+  <si>
+    <t>PR.KOL.09.</t>
+  </si>
+  <si>
+    <t>Kolekcijas rediģēšana</t>
+  </si>
+  <si>
+    <t>Jaunuma dzēšanas atcelšana</t>
+  </si>
+  <si>
+    <t>TP.BB.J.DZE.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOM.I.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOM.I.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOM.IER.01.</t>
+  </si>
+  <si>
+    <t>Jauna komentāra ierakstīšana</t>
+  </si>
+  <si>
+    <t>Pastāvoša stāsta ierakstīšana izmainot aprakstu un sastāvu</t>
+  </si>
+  <si>
+    <t>Pastāvoša stāsta ierakstīšana izmainot sastāvu</t>
+  </si>
+  <si>
+    <t>Pastāvoša stāsta ierakstīšana izmainot aprakstu</t>
+  </si>
+  <si>
+    <t>Pastāvoša stāsta rediģētā satura iesūtīšana</t>
+  </si>
+  <si>
+    <t>Pastāvoša stāsta rediģētā apraksta iesūtīšana</t>
+  </si>
+  <si>
+    <t>Pastāvoša stāsta rediģētā satura un apraksta iesūtīšana</t>
+  </si>
+  <si>
+    <t>TP.BB.S.R.03.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.R.04.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.R.05.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.R.06.</t>
+  </si>
+  <si>
+    <t>TP.BB.S.R.07.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOM.IES.01.</t>
+  </si>
+  <si>
+    <t>Jauna komentāra iesūtīšana</t>
+  </si>
+  <si>
+    <t>TP.BB.KOM.DZE.01.</t>
+  </si>
+  <si>
+    <t>Komentāra izdzēšana kā komentāra autors</t>
+  </si>
+  <si>
+    <t>Komentāra izdzēšana kā administrators</t>
+  </si>
+  <si>
+    <t>TP.BB.KOM.DZE.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.J.DZE.03.</t>
+  </si>
+  <si>
+    <t>Jaunuma dzēšana kā administrators</t>
+  </si>
+  <si>
+    <t>Jaunuma dzēšana kā jaunuma autors</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.I.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.I.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.I.03.</t>
+  </si>
+  <si>
+    <t>Individuālas kolekcijas sadaļas ielāde</t>
+  </si>
+  <si>
+    <t>Individuālas kolekcijas saņemšanas no datubāzes</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.I.04.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.DZE.01.</t>
+  </si>
+  <si>
+    <t>Kolekcijas izdzēšana kā administrators</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.DZE.02.</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.IES.01.</t>
+  </si>
+  <si>
+    <t>Jaunas kolekcijas iesūtīšana</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.IES.02.</t>
+  </si>
+  <si>
+    <t>Jaunas kolekcijas ierakstīšana</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.R.01.</t>
+  </si>
+  <si>
+    <t>Kolekcijas satura rediģēšana</t>
+  </si>
+  <si>
+    <t>Kolekcijas rediģēšanas atcelšana</t>
+  </si>
+  <si>
+    <t>TP.BB.KOL.R.02.</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.S.01.</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.S.02.</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.L.01.</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Lietotājs</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.L.02.</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.S.03.</t>
+  </si>
+  <si>
+    <t>Stāsta pievienošana kolekcijai kā kolekcijas dalībnieks</t>
+  </si>
+  <si>
+    <t>Stāsta pievienošana kolekcijai kā kolekcijas īpašnieks</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.S.04.</t>
+  </si>
+  <si>
+    <t>Stāsta noņemšana no kolekcijas kā kolekcijas īpašnieks</t>
+  </si>
+  <si>
+    <t>Stāsta noņemšana no kolekcijas kā kolekcijas dalībnieks</t>
+  </si>
+  <si>
+    <t>Lietotāja pievienošana kolekcijai kā kolekcijas īpašnieks</t>
+  </si>
+  <si>
+    <t>Lietotāja pievienošana kolekcijai kā kolekcijas dalībnieks</t>
+  </si>
+  <si>
+    <t>Lietotāja noņemšana no kolekcijas kā noņemamais lietotājs</t>
+  </si>
+  <si>
+    <t>Lietotāja noņemšana no kolekcijas kā kolekcijas īpašnieks</t>
+  </si>
+  <si>
+    <t>Kolekcijas īpašnieka noņemšana no kolekcijas kā kolekcijas īpašnieks</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.L.03.</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.L.04.</t>
+  </si>
+  <si>
+    <t>TP..BB.KOL.R.L.05.</t>
+  </si>
+  <si>
+    <t>Kolekcijas izdzēšana kā kolekcijas īpašnieks</t>
+  </si>
+  <si>
+    <t>TP.BB.A.I.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.A.I.02.</t>
+  </si>
+  <si>
+    <t>Administratora sadaļas ielāde kā administrators</t>
+  </si>
+  <si>
+    <t>Administratora sadaļas ielāde kā lietotājs bez administratora spējām</t>
+  </si>
+  <si>
+    <t>TP.BB.A.I.03.</t>
+  </si>
+  <si>
+    <t>Administratora statistikas saņemšana no datubāzes</t>
+  </si>
+  <si>
+    <t>Administratora profila skata ielāde</t>
+  </si>
+  <si>
+    <t>TP.BB.A.R.K.01.</t>
+  </si>
+  <si>
+    <t>TP.BB.A.I.04.</t>
+  </si>
+  <si>
+    <t>TP.BB.A.R.K.02.</t>
+  </si>
+  <si>
+    <t>Atvērta tīmekļvietne, nav aktīvas sesijas</t>
+  </si>
+  <si>
+    <t>Atvērta tīmekļvietne, nav aktīvas sesijas, izpildīts testpiemērs TP.BB.SES.04.</t>
+  </si>
+  <si>
+    <t>Atvērta tīmekļvietnes mājaslapa, pastāv aktīva sesija</t>
+  </si>
+  <si>
+    <t>Atvērta tīmekļvietnes mājaslapa, pastāv aktīva lietotāja sesija ar administratora spējām</t>
+  </si>
+  <si>
+    <t>Atvērta tīmekļvietnes "Login" lapa, nav aktīvas sesijas</t>
   </si>
 </sst>
 </file>
@@ -940,7 +1313,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1002,6 +1375,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1323,13 +1702,16 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+    <sheetView workbookViewId="2">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1457,105 +1839,121 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>7</v>
+        <v>238</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>331</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1576,15 +1974,17 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="1">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1694,7 +2094,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1726,7 +2126,7 @@
         <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1734,7 +2134,7 @@
         <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1742,198 +2142,286 @@
         <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>214</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="9"/>
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>201</v>
+        <v>256</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>207</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>198</v>
-      </c>
+      <c r="A23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="B26" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="9"/>
+      <c r="A27" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>204</v>
+        <v>253</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>209</v>
+        <v>273</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>212</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>213</v>
+      <c r="A31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="9"/>
+      <c r="A33" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="9"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>231</v>
-      </c>
+      <c r="A43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="9"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="B48" s="9"/>
+      <c r="B54" s="9"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>248</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1946,13 +2434,19 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="2">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2048,7 +2542,9 @@
       <c r="B5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>363</v>
+      </c>
       <c r="D5" s="8" t="s">
         <v>113</v>
       </c>
@@ -2068,7 +2564,9 @@
       <c r="B6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>363</v>
+      </c>
       <c r="D6" s="8" t="s">
         <v>114</v>
       </c>
@@ -2077,7 +2575,7 @@
       <c r="G6" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2088,7 +2586,9 @@
       <c r="B7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>363</v>
+      </c>
       <c r="D7" s="8" t="s">
         <v>115</v>
       </c>
@@ -2097,7 +2597,7 @@
       <c r="G7" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2108,14 +2608,16 @@
       <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="D8" s="11" t="s">
         <v>161</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2126,14 +2628,16 @@
       <c r="B9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="D9" s="8" t="s">
         <v>140</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2144,14 +2648,16 @@
       <c r="B10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="D10" s="8" t="s">
         <v>141</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2162,14 +2668,16 @@
       <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="D11" s="8" t="s">
         <v>144</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="11" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2180,29 +2688,40 @@
       <c r="B12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>360</v>
+      </c>
       <c r="D12" s="8" t="s">
         <v>177</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="H12" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
+      <c r="H13" s="11" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>44</v>
-      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -2226,65 +2745,71 @@
       <c r="B16" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="C16" s="8" t="s">
+        <v>361</v>
+      </c>
       <c r="D16" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="H16" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="C17" s="8" t="s">
+        <v>362</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="H17" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="H18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="H19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -2302,7 +2827,7 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>181</v>
+        <v>291</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -2311,7 +2836,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>179</v>
       </c>
@@ -2320,318 +2845,385 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>184</v>
+        <v>292</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>170</v>
+        <v>297</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>183</v>
+        <v>293</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>180</v>
+        <v>298</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
-        <v>182</v>
+        <v>296</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>171</v>
+        <v>299</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="11" t="s">
-        <v>65</v>
+      <c r="D25" s="8" t="s">
+        <v>294</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>172</v>
+        <v>300</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="11" t="s">
-        <v>66</v>
+      <c r="D26" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="11" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>173</v>
+        <v>301</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="11" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="11" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="A30" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
+      <c r="A31" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="H31" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
+      <c r="A32" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+      <c r="H32" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="D33" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+      <c r="H33" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>187</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
+      <c r="H34" s="11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
+      <c r="A36" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
+    <row r="38" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
+      <c r="D38" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+    <row r="39" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="D39" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
+    <row r="40" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="D40" s="11" t="s">
+        <v>264</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
+    <row r="41" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>272</v>
+      </c>
       <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="D41" s="8" t="s">
+        <v>266</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="42" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-    </row>
-    <row r="43" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>109</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C43" s="8"/>
       <c r="D43" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>18</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
+      <c r="D44" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
+      <c r="A45" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
@@ -2644,91 +3236,126 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-    </row>
-    <row r="48" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>166</v>
+        <v>275</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>101</v>
+        <v>208</v>
       </c>
       <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
+      <c r="D48" s="11" t="s">
+        <v>208</v>
+      </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>167</v>
+        <v>276</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>50</v>
+        <v>202</v>
       </c>
       <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
+      <c r="D49" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
+      <c r="A50" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>279</v>
+      </c>
       <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
+      <c r="D50" s="8" t="s">
+        <v>279</v>
+      </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+    <row r="51" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>280</v>
+      </c>
       <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
+      <c r="D51" s="8" t="s">
+        <v>280</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
+    <row r="52" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+    </row>
+    <row r="53" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>282</v>
+      </c>
       <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
+      <c r="D53" s="8" t="s">
+        <v>309</v>
+      </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
+      <c r="A54" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
@@ -2771,29 +3398,873 @@
       <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
+      <c r="A60" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>214</v>
+      </c>
       <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
+      <c r="D60" s="8" t="s">
+        <v>214</v>
+      </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
     </row>
+    <row r="61" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+    </row>
+    <row r="64" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+    </row>
+    <row r="65" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="24"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+    </row>
+    <row r="69" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+    </row>
+    <row r="70" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+    </row>
+    <row r="71" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+    </row>
+    <row r="74" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+    </row>
+    <row r="75" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+    </row>
+    <row r="77" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+    </row>
+    <row r="78" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+    </row>
+    <row r="79" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C79" s="8"/>
+      <c r="D79" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+    </row>
+    <row r="80" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+    </row>
+    <row r="81" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+    </row>
+    <row r="82" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+    </row>
+    <row r="83" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+    </row>
+    <row r="84" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+    </row>
+    <row r="85" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" s="8"/>
+      <c r="D85" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+    </row>
+    <row r="86" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="25"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C89" s="8"/>
+      <c r="D89" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+    </row>
+    <row r="91" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+    </row>
+    <row r="93" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C97" s="8"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="8"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="8"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="8"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C105" s="8"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C107" s="8"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="8"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
+    </row>
+    <row r="109" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+      <c r="G109" s="8"/>
+      <c r="H109" s="8"/>
+    </row>
+    <row r="110" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B110" s="22"/>
+      <c r="C110" s="22"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="22"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22"/>
+      <c r="H110" s="22"/>
+    </row>
+    <row r="111" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A111" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H111" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="8"/>
+      <c r="H112" s="8"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="12"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="8"/>
+      <c r="H114" s="8"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="12"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+      <c r="G115" s="12"/>
+      <c r="H115" s="12"/>
+    </row>
+    <row r="116" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+      <c r="G117" s="8"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="8"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="8"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="12"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
+      <c r="G122" s="12"/>
+      <c r="H122" s="12"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="8"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+      <c r="F124" s="8"/>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="8"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8"/>
+      <c r="F125" s="8"/>
+      <c r="G125" s="8"/>
+      <c r="H125" s="8"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
+      <c r="F126" s="8"/>
+      <c r="G126" s="8"/>
+      <c r="H126" s="8"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+      <c r="F128" s="8"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A110:H110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2814,7 +4285,11 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Reset to functional code with minimal improvements
</commit_message>
<xml_diff>
--- a/Laudobele Telma Testesanas Dokumentacija.xlsx
+++ b/Laudobele Telma Testesanas Dokumentacija.xlsx
@@ -8,11 +8,11 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telmy\OneDrive\school\final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA4DCB4-B42D-4FB4-8474-6568DF986072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770C2536-105E-489F-A670-3A55AFE3B8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="0" windowWidth="16815" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
-    <workbookView xWindow="20955" yWindow="0" windowWidth="7800" windowHeight="15600" activeTab="1" xr2:uid="{56FCC86A-F332-49E3-B109-B86D43588ADF}"/>
-    <workbookView xWindow="16770" yWindow="60" windowWidth="4530" windowHeight="15480" firstSheet="2" activeTab="2" xr2:uid="{BCE1B89D-1D04-49A8-9071-0D8B36985319}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="15540" firstSheet="1" activeTab="2" xr2:uid="{EF473932-1A0F-402F-B745-DD1FD387BA71}"/>
+    <workbookView xWindow="22365" yWindow="105" windowWidth="6405" windowHeight="15540" activeTab="1" xr2:uid="{56FCC86A-F332-49E3-B109-B86D43588ADF}"/>
+    <workbookView minimized="1" xWindow="12750" yWindow="660" windowWidth="7575" windowHeight="15540" firstSheet="2" activeTab="2" xr2:uid="{BCE1B89D-1D04-49A8-9071-0D8B36985319}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -1361,6 +1361,12 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1375,12 +1381,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1722,34 +1722,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="22"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="22"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1768,10 +1768,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -2438,14 +2438,16 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="2">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="2">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2488,16 +2490,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -2929,7 +2931,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>170</v>
       </c>
@@ -3236,14 +3238,14 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
@@ -3514,14 +3516,14 @@
       <c r="H66" s="8"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="24"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="24"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
@@ -3826,14 +3828,14 @@
       <c r="H86" s="8"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="24"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
@@ -4047,16 +4049,16 @@
       <c r="H109" s="8"/>
     </row>
     <row r="110" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B110" s="22"/>
-      <c r="C110" s="22"/>
-      <c r="D110" s="22"/>
-      <c r="E110" s="22"/>
-      <c r="F110" s="22"/>
-      <c r="G110" s="22"/>
-      <c r="H110" s="22"/>
+      <c r="B110" s="24"/>
+      <c r="C110" s="24"/>
+      <c r="D110" s="24"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="24"/>
+      <c r="H110" s="24"/>
     </row>
     <row r="111" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">

</xml_diff>